<commit_message>
Log based corrections - text highlighting,
</commit_message>
<xml_diff>
--- a/Documents/FromCustomer/15Mar2017/DDAS Issue Log_15Mar17_Updated.xlsx
+++ b/Documents/FromCustomer/15Mar2017/DDAS Issue Log_15Mar17_Updated.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="150" windowWidth="16275" windowHeight="5715" tabRatio="582"/>
+    <workbookView xWindow="360" yWindow="150" windowWidth="16275" windowHeight="5715" tabRatio="312"/>
   </bookViews>
   <sheets>
     <sheet name="DDAS Issue Logs" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="133">
   <si>
     <t>Issue Date</t>
   </si>
@@ -292,9 +292,6 @@
     <t>Please provide more details and indicate the Project Number + Principal Investigator, Site Source and expected result.</t>
   </si>
   <si>
-    <t>1. Date of Action: is available and can be included in the display.  2. 'Code'  - not clear how to extract the code.  3. 1128(b)14 / 1128b14, the data downloaded from the site has a slightly different format from the one displayed on the web site.  It is difficult to selectively modify the format.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Please identify the filters required for all the pages.  A minimal number of filters will make the page more usable.  </t>
   </si>
   <si>
@@ -331,15 +328,9 @@
     <t>check:Pradeep/Patrick</t>
   </si>
   <si>
-    <t>Pradeep - list out all the web links and request Icon for info.</t>
-  </si>
-  <si>
     <t>Done</t>
   </si>
   <si>
-    <t>check: Pradeep</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pradeep   </t>
   </si>
   <si>
@@ -349,13 +340,100 @@
     <t>check:patrick / pradeep</t>
   </si>
   <si>
-    <t>patrick / pradeep</t>
-  </si>
-  <si>
     <t>patrick</t>
   </si>
   <si>
     <t>Pradeep</t>
+  </si>
+  <si>
+    <t>Generated Compliance Form ? Identified, will be corrected.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Date of Action: is available and can be included in the display.  </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2. 'Code'  - not clear how to extract the code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.  3. 1128(b)14 / 1128b14, the data downloaded from the site has a slightly different format from the one displayed on the web site.  It is difficult to selectively modify the format.</t>
+    </r>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Corrected.</t>
+  </si>
+  <si>
+    <t>to be tested</t>
+  </si>
+  <si>
+    <t>Require some Web Urls from ICON</t>
+  </si>
+  <si>
+    <t>ICON</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>No solution yet</t>
+  </si>
+  <si>
+    <t>ICOn to provide details</t>
+  </si>
+  <si>
+    <t>Request ICOn for details</t>
+  </si>
+  <si>
+    <t>Signle Component result required.  Pros and Cons of Single Component result to be explained to ICON</t>
+  </si>
+  <si>
+    <t>Info to ICON: No of matches for single component result</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Info awaited from ICON</t>
+  </si>
+  <si>
+    <t>To be tested.</t>
+  </si>
+  <si>
+    <t>Process explained.  No further action required.</t>
+  </si>
+  <si>
+    <t>Sort Order: Inv (PI, SI), Site No, Date of Action</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Pradeep: email</t>
+  </si>
+  <si>
+    <t>Comp Form - new property :NameToSearch</t>
+  </si>
+  <si>
+    <t>require list of special charcters from ICON</t>
+  </si>
+  <si>
+    <t>Inf required</t>
   </si>
 </sst>
 </file>
@@ -365,7 +443,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]dd\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,8 +475,15 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -408,6 +493,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,7 +534,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -475,14 +572,46 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -535,6 +664,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+      <alignment textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -688,19 +818,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J31" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10">
-  <autoFilter ref="A1:J31"/>
-  <tableColumns count="10">
-    <tableColumn id="1" name="Serial No." dataDxfId="9"/>
-    <tableColumn id="2" name="Issue Date" dataDxfId="8"/>
-    <tableColumn id="3" name="Title" dataDxfId="7"/>
-    <tableColumn id="8" name="Issue Description" dataDxfId="6"/>
-    <tableColumn id="9" name="Category" dataDxfId="5"/>
-    <tableColumn id="4" name="Status" dataDxfId="4"/>
-    <tableColumn id="5" name="Action" dataDxfId="3"/>
-    <tableColumn id="6" name="Severity" dataDxfId="2"/>
-    <tableColumn id="10" name="Close Date" dataDxfId="1"/>
-    <tableColumn id="7" name="Column1" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L31" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
+  <autoFilter ref="A1:L31">
+    <filterColumn colId="9">
+      <filters>
+        <filter val="Patrick"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="10">
+      <filters>
+        <filter val="Pending"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="12">
+    <tableColumn id="1" name="Serial No." dataDxfId="11"/>
+    <tableColumn id="2" name="Issue Date" dataDxfId="10"/>
+    <tableColumn id="3" name="Title" dataDxfId="9"/>
+    <tableColumn id="8" name="Issue Description" dataDxfId="8"/>
+    <tableColumn id="9" name="Category" dataDxfId="7"/>
+    <tableColumn id="4" name="Status" dataDxfId="6"/>
+    <tableColumn id="5" name="Action" dataDxfId="5"/>
+    <tableColumn id="6" name="Severity" dataDxfId="4"/>
+    <tableColumn id="10" name="Close Date" dataDxfId="3"/>
+    <tableColumn id="7" name="Column1" dataDxfId="2"/>
+    <tableColumn id="11" name="Column2" dataDxfId="1"/>
+    <tableColumn id="12" name="Column3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -885,10 +1028,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,14 +1045,14 @@
     <col min="4" max="4" width="28.25" style="3" customWidth="1"/>
     <col min="5" max="5" width="14.75" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5" style="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.25" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.125" style="11" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="20.5" style="3" customWidth="1"/>
     <col min="12" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -935,10 +1081,16 @@
         <v>6</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -957,7 +1109,7 @@
       <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>87</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -966,7 +1118,7 @@
       <c r="I2" s="10"/>
       <c r="J2" s="13"/>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" s="2" customFormat="1" ht="180" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -985,23 +1137,28 @@
       <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="4" t="s">
         <v>88</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="10"/>
-      <c r="J3" s="13"/>
-    </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="J3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="2" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="5">
         <v>42809</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="17" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="6" t="s">
@@ -1013,7 +1170,7 @@
       <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="4" t="s">
         <v>89</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -1021,10 +1178,13 @@
       </c>
       <c r="I4" s="10"/>
       <c r="J4" s="13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1054,14 +1214,14 @@
       </c>
       <c r="J5" s="13"/>
     </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" s="2" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="5">
         <v>42809</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="17" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -1073,7 +1233,7 @@
       <c r="F6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="4" t="s">
         <v>78</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -1081,10 +1241,13 @@
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1103,7 +1266,7 @@
       <c r="F7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="4" t="s">
         <v>79</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -1111,17 +1274,20 @@
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="5">
         <v>42809</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="6" t="s">
@@ -1133,23 +1299,28 @@
       <c r="F8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="4" t="s">
         <v>81</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I8" s="10"/>
-      <c r="J8" s="13"/>
-    </row>
-    <row r="9" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="J8" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="2" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="5">
         <v>42809</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="16" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="6" t="s">
@@ -1161,25 +1332,31 @@
       <c r="F9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="4" t="s">
         <v>79</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I9" s="10"/>
-      <c r="J9" s="15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="J9" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="2" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="5">
         <v>42809</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="16" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="6" t="s">
@@ -1191,7 +1368,7 @@
       <c r="F10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="4" t="s">
         <v>82</v>
       </c>
       <c r="H10" s="2" t="s">
@@ -1199,8 +1376,11 @@
       </c>
       <c r="I10" s="10"/>
       <c r="J10" s="13"/>
-    </row>
-    <row r="11" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="L10" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1219,7 +1399,7 @@
       <c r="F11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H11" s="2" t="s">
@@ -1227,17 +1407,23 @@
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="5">
         <v>42809</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="17" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="6" t="s">
@@ -1249,7 +1435,7 @@
       <c r="F12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="4" t="s">
         <v>84</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -1257,17 +1443,20 @@
       </c>
       <c r="I12" s="10"/>
       <c r="J12" s="13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="2" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="5">
         <v>42809</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="16" t="s">
         <v>35</v>
       </c>
       <c r="D13" s="6" t="s">
@@ -1279,25 +1468,28 @@
       <c r="F13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="4" t="s">
         <v>85</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>37</v>
       </c>
       <c r="I13" s="10"/>
-      <c r="J13" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="J13" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="2" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="5">
         <v>42809</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
       <c r="D14" s="6" t="s">
@@ -1309,23 +1501,28 @@
       <c r="F14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="4" t="s">
         <v>90</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>37</v>
       </c>
       <c r="I14" s="10"/>
-      <c r="J14" s="13"/>
-    </row>
-    <row r="15" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="J14" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="2" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="5">
         <v>42809</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="17" t="s">
         <v>35</v>
       </c>
       <c r="D15" s="6" t="s">
@@ -1337,16 +1534,24 @@
       <c r="F15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="4" t="s">
         <v>91</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>37</v>
       </c>
       <c r="I15" s="10"/>
-      <c r="J15" s="13"/>
-    </row>
-    <row r="16" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="J15" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="2" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1365,23 +1570,28 @@
       <c r="F16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="4" t="s">
         <v>80</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I16" s="10"/>
-      <c r="J16" s="13"/>
-    </row>
-    <row r="17" spans="1:10" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+      <c r="J16" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="2" customFormat="1" ht="180" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="5">
         <v>42809</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="16" t="s">
         <v>40</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -1393,18 +1603,21 @@
       <c r="F17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>92</v>
+      <c r="G17" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I17" s="10"/>
       <c r="J17" s="13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="2" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1423,23 +1636,26 @@
       <c r="F18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>93</v>
+      <c r="G18" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I18" s="10"/>
       <c r="J18" s="13"/>
-    </row>
-    <row r="19" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="K18" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="2" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="5">
         <v>42809</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="17" t="s">
         <v>43</v>
       </c>
       <c r="D19" s="6" t="s">
@@ -1451,7 +1667,7 @@
       <c r="F19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="4" t="s">
         <v>86</v>
       </c>
       <c r="H19" s="2" t="s">
@@ -1459,10 +1675,13 @@
       </c>
       <c r="I19" s="10"/>
       <c r="J19" s="13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1481,7 +1700,7 @@
       <c r="F20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="4" t="s">
         <v>79</v>
       </c>
       <c r="H20" s="2" t="s">
@@ -1489,10 +1708,13 @@
       </c>
       <c r="I20" s="10"/>
       <c r="J20" s="13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="2" customFormat="1" ht="255" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1511,18 +1733,21 @@
       <c r="F21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>94</v>
+      <c r="G21" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>37</v>
       </c>
       <c r="I21" s="10"/>
-      <c r="J21" s="13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="J21" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="2" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1541,13 +1766,21 @@
       <c r="F22" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="4" t="s">
         <v>80</v>
       </c>
       <c r="I22" s="10"/>
-      <c r="J22" s="13"/>
-    </row>
-    <row r="23" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="J22" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1566,15 +1799,18 @@
       <c r="F23" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>95</v>
+      <c r="G23" s="4" t="s">
+        <v>94</v>
       </c>
       <c r="I23" s="10"/>
       <c r="J23" s="13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="2" customFormat="1" ht="120" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1593,16 +1829,18 @@
       <c r="F24" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>96</v>
+      <c r="G24" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>37</v>
       </c>
       <c r="I24" s="10"/>
-      <c r="J24" s="13"/>
-    </row>
-    <row r="25" spans="1:10" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+      <c r="J24" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="2" customFormat="1" ht="180" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1621,16 +1859,19 @@
       <c r="F25" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>97</v>
+      <c r="G25" s="4" t="s">
+        <v>96</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>37</v>
       </c>
       <c r="I25" s="10"/>
       <c r="J25" s="13"/>
-    </row>
-    <row r="26" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="K25" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1649,16 +1890,21 @@
       <c r="F26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="4" t="s">
         <v>80</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>37</v>
       </c>
       <c r="I26" s="10"/>
-      <c r="J26" s="13"/>
-    </row>
-    <row r="27" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="J26" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1677,16 +1923,21 @@
       <c r="F27" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>98</v>
+      <c r="G27" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I27" s="10"/>
-      <c r="J27" s="13"/>
-    </row>
-    <row r="28" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="J27" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1705,16 +1956,21 @@
       <c r="F28" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>99</v>
+      <c r="G28" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I28" s="10"/>
-      <c r="J28" s="13"/>
-    </row>
-    <row r="29" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="J28" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="2" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1733,16 +1989,21 @@
       <c r="F29" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>100</v>
+      <c r="G29" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I29" s="10"/>
-      <c r="J29" s="13"/>
-    </row>
-    <row r="30" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="J29" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1761,7 +2022,7 @@
       <c r="F30" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H30" s="2" t="s">
@@ -1769,10 +2030,13 @@
       </c>
       <c r="I30" s="10"/>
       <c r="J30" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1791,20 +2055,24 @@
       <c r="F31" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G31" s="2" t="s">
-        <v>101</v>
+      <c r="G31" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I31" s="10"/>
       <c r="J31" s="13" t="s">
-        <v>113</v>
+        <v>109</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="51" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>

<commit_message>
datepicker - date-input component tested, working ok.
</commit_message>
<xml_diff>
--- a/Documents/FromCustomer/15Mar2017/DDAS Issue Log_15Mar17_Updated.xlsx
+++ b/Documents/FromCustomer/15Mar2017/DDAS Issue Log_15Mar17_Updated.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="150" windowWidth="16275" windowHeight="5715" tabRatio="312"/>
+    <workbookView xWindow="7095" yWindow="150" windowWidth="13320" windowHeight="7710" tabRatio="217"/>
   </bookViews>
   <sheets>
     <sheet name="DDAS Issue Logs" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="131">
   <si>
     <t>Issue Date</t>
   </si>
@@ -325,9 +325,6 @@
     <t>Column1</t>
   </si>
   <si>
-    <t>check:Pradeep/Patrick</t>
-  </si>
-  <si>
     <t>Done</t>
   </si>
   <si>
@@ -344,9 +341,6 @@
   </si>
   <si>
     <t>Pradeep</t>
-  </si>
-  <si>
-    <t>Generated Compliance Form ? Identified, will be corrected.</t>
   </si>
   <si>
     <r>
@@ -379,9 +373,6 @@
     <t>Corrected.</t>
   </si>
   <si>
-    <t>to be tested</t>
-  </si>
-  <si>
     <t>Require some Web Urls from ICON</t>
   </si>
   <si>
@@ -400,9 +391,6 @@
     <t>Request ICOn for details</t>
   </si>
   <si>
-    <t>Signle Component result required.  Pros and Cons of Single Component result to be explained to ICON</t>
-  </si>
-  <si>
     <t>Info to ICON: No of matches for single component result</t>
   </si>
   <si>
@@ -424,9 +412,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Pradeep: email</t>
-  </si>
-  <si>
     <t>Comp Form - new property :NameToSearch</t>
   </si>
   <si>
@@ -434,6 +419,15 @@
   </si>
   <si>
     <t>Inf required</t>
+  </si>
+  <si>
+    <t>No error found. User Marked the review completed before Live Extration is completed</t>
+  </si>
+  <si>
+    <t>No error found. Spelling mistake in input. Explained.</t>
+  </si>
+  <si>
+    <t>Pt 1 and 2 corrected. Pt 3 Not feasible, explained</t>
   </si>
 </sst>
 </file>
@@ -819,18 +813,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L31" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
-  <autoFilter ref="A1:L31">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="Patrick"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="10">
-      <filters>
-        <filter val="Pending"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:L31"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Serial No." dataDxfId="11"/>
     <tableColumn id="2" name="Issue Date" dataDxfId="10"/>
@@ -1033,8 +1016,8 @@
   </sheetPr>
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,20 +1067,20 @@
         <v>102</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="5">
         <v>42809</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
@@ -1116,16 +1099,18 @@
         <v>11</v>
       </c>
       <c r="I2" s="10"/>
-      <c r="J2" s="13"/>
-    </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="180" hidden="1" x14ac:dyDescent="0.2">
+      <c r="J2" s="13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="2" customFormat="1" ht="180" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="5">
         <v>42809</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="16" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="6" t="s">
@@ -1145,13 +1130,13 @@
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="2" customFormat="1" ht="150" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1181,10 +1166,10 @@
         <v>101</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1214,7 +1199,7 @@
       </c>
       <c r="J5" s="13"/>
     </row>
-    <row r="6" spans="1:12" s="2" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1244,17 +1229,17 @@
         <v>101</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="5">
         <v>42809</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="17" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -1274,13 +1259,13 @@
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="13" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1307,13 +1292,13 @@
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="2" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="2" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1340,16 +1325,16 @@
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="4" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="2" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1377,17 +1362,17 @@
       <c r="I10" s="10"/>
       <c r="J10" s="13"/>
       <c r="L10" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="5">
         <v>42809</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="17" t="s">
         <v>60</v>
       </c>
       <c r="D11" s="6" t="s">
@@ -1410,13 +1395,13 @@
         <v>101</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1443,20 +1428,20 @@
       </c>
       <c r="I12" s="10"/>
       <c r="J12" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="2" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="5">
         <v>42809</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="17" t="s">
         <v>35</v>
       </c>
       <c r="D13" s="6" t="s">
@@ -1476,20 +1461,23 @@
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="2" t="s">
-        <v>129</v>
+        <v>108</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="2" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="5">
         <v>42809</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="17" t="s">
         <v>35</v>
       </c>
       <c r="D14" s="6" t="s">
@@ -1509,13 +1497,16 @@
       </c>
       <c r="I14" s="10"/>
       <c r="J14" s="2" t="s">
-        <v>129</v>
+        <v>108</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="2" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1542,23 +1533,23 @@
       </c>
       <c r="I15" s="10"/>
       <c r="J15" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K15" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>121</v>
-      </c>
       <c r="L15" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="2" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="5">
         <v>42809</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="16" t="s">
         <v>39</v>
       </c>
       <c r="D16" s="6" t="s">
@@ -1578,20 +1569,20 @@
       </c>
       <c r="I16" s="10"/>
       <c r="J16" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="2" customFormat="1" ht="180" hidden="1" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="2" customFormat="1" ht="180" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="5">
         <v>42809</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="17" t="s">
         <v>40</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -1604,20 +1595,20 @@
         <v>9</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I17" s="10"/>
       <c r="J17" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" s="2" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1645,10 +1636,10 @@
       <c r="I18" s="10"/>
       <c r="J18" s="13"/>
       <c r="K18" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" s="2" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1675,13 +1666,13 @@
       </c>
       <c r="I19" s="10"/>
       <c r="J19" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1708,20 +1699,20 @@
       </c>
       <c r="I20" s="10"/>
       <c r="J20" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" s="2" customFormat="1" ht="255" hidden="1" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="2" customFormat="1" ht="255" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="5">
         <v>42809</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="17" t="s">
         <v>47</v>
       </c>
       <c r="D21" s="6" t="s">
@@ -1741,20 +1732,20 @@
       </c>
       <c r="I21" s="10"/>
       <c r="J21" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" s="2" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="5">
         <v>42809</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="16" t="s">
         <v>74</v>
       </c>
       <c r="D22" s="6" t="s">
@@ -1771,13 +1762,13 @@
       </c>
       <c r="I22" s="10"/>
       <c r="J22" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="K22" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L22" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
@@ -1787,7 +1778,7 @@
       <c r="B23" s="5">
         <v>42809</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="17" t="s">
         <v>50</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -1804,20 +1795,20 @@
       </c>
       <c r="I23" s="10"/>
       <c r="J23" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" s="2" customFormat="1" ht="120" hidden="1" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="5">
         <v>42809</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="16" t="s">
         <v>51</v>
       </c>
       <c r="D24" s="6" t="s">
@@ -1837,17 +1828,17 @@
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" s="2" customFormat="1" ht="180" hidden="1" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="2" customFormat="1" ht="180" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="5">
         <v>42809</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="17" t="s">
         <v>52</v>
       </c>
       <c r="D25" s="6" t="s">
@@ -1868,10 +1859,10 @@
       <c r="I25" s="10"/>
       <c r="J25" s="13"/>
       <c r="K25" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1898,10 +1889,10 @@
       </c>
       <c r="I26" s="10"/>
       <c r="J26" s="2" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:12" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.2">
@@ -1934,7 +1925,7 @@
         <v>101</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
@@ -1967,10 +1958,10 @@
         <v>101</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" s="2" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1997,13 +1988,13 @@
       </c>
       <c r="I29" s="10"/>
       <c r="J29" s="2" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2030,13 +2021,13 @@
       </c>
       <c r="I30" s="10"/>
       <c r="J30" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -2063,10 +2054,10 @@
       </c>
       <c r="I31" s="10"/>
       <c r="J31" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WebSite - angular changes
</commit_message>
<xml_diff>
--- a/Documents/FromCustomer/15Mar2017/DDAS Issue Log_15Mar17_Updated.xlsx
+++ b/Documents/FromCustomer/15Mar2017/DDAS Issue Log_15Mar17_Updated.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="7095" yWindow="150" windowWidth="13320" windowHeight="7710" tabRatio="217"/>
+    <workbookView xWindow="7095" yWindow="150" windowWidth="13320" windowHeight="7710" tabRatio="236"/>
   </bookViews>
   <sheets>
     <sheet name="DDAS Issue Logs" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="132">
   <si>
     <t>Issue Date</t>
   </si>
@@ -428,6 +428,9 @@
   </si>
   <si>
     <t>Pt 1 and 2 corrected. Pt 3 Not feasible, explained</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pradeep </t>
   </si>
 </sst>
 </file>
@@ -1016,8 +1019,8 @@
   </sheetPr>
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,7 +1083,7 @@
       <c r="B2" s="5">
         <v>42809</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="17" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
@@ -1100,7 +1103,10 @@
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="13" t="s">
-        <v>108</v>
+        <v>131</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" ht="180" x14ac:dyDescent="0.2">
@@ -1679,7 +1685,7 @@
       <c r="B20" s="5">
         <v>42809</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="17" t="s">
         <v>45</v>
       </c>
       <c r="D20" s="6" t="s">
@@ -1745,7 +1751,7 @@
       <c r="B22" s="5">
         <v>42809</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="17" t="s">
         <v>74</v>
       </c>
       <c r="D22" s="6" t="s">
@@ -1765,7 +1771,7 @@
         <v>101</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>123</v>
@@ -1829,6 +1835,9 @@
       <c r="I24" s="10"/>
       <c r="J24" s="2" t="s">
         <v>108</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="2" customFormat="1" ht="180" x14ac:dyDescent="0.2">
@@ -2001,7 +2010,7 @@
       <c r="B30" s="5">
         <v>42809</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="17" t="s">
         <v>71</v>
       </c>
       <c r="D30" s="6" t="s">
@@ -2024,7 +2033,7 @@
         <v>108</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
@@ -2034,7 +2043,7 @@
       <c r="B31" s="5">
         <v>42809</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="17" t="s">
         <v>72</v>
       </c>
       <c r="D31" s="6" t="s">
@@ -2057,7 +2066,7 @@
         <v>108</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug: Roll up incorrect.   -- corrected. Corrections in Site Source Corrections in Country specific sites
</commit_message>
<xml_diff>
--- a/Documents/FromCustomer/15Mar2017/DDAS Issue Log_15Mar17_Updated.xlsx
+++ b/Documents/FromCustomer/15Mar2017/DDAS Issue Log_15Mar17_Updated.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="126">
   <si>
     <t>Issue Date</t>
   </si>
@@ -319,28 +319,7 @@
     <t>Will be provided.  We may require more details and will request for the same.</t>
   </si>
   <si>
-    <t>Patrick</t>
-  </si>
-  <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>Done</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pradeep   </t>
-  </si>
-  <si>
-    <t>done</t>
-  </si>
-  <si>
-    <t>check:patrick / pradeep</t>
-  </si>
-  <si>
-    <t>patrick</t>
-  </si>
-  <si>
-    <t>Pradeep</t>
   </si>
   <si>
     <r>
@@ -373,9 +352,6 @@
     <t>Corrected.</t>
   </si>
   <si>
-    <t>Require some Web Urls from ICON</t>
-  </si>
-  <si>
     <t>ICON</t>
   </si>
   <si>
@@ -412,15 +388,9 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Comp Form - new property :NameToSearch</t>
-  </si>
-  <si>
     <t>require list of special charcters from ICON</t>
   </si>
   <si>
-    <t>Inf required</t>
-  </si>
-  <si>
     <t>No error found. User Marked the review completed before Live Extration is completed</t>
   </si>
   <si>
@@ -430,7 +400,19 @@
     <t>Pt 1 and 2 corrected. Pt 3 Not feasible, explained</t>
   </si>
   <si>
-    <t xml:space="preserve">Pradeep </t>
+    <t>Not completed.  Application design changes in progress to incporate First Name, Middle Name and Last Name and these changes are exprected meet this requirement.</t>
+  </si>
+  <si>
+    <t>Corrected</t>
+  </si>
+  <si>
+    <t>No solution available.</t>
+  </si>
+  <si>
+    <t>Done.  It is now possible to add a finding under Findings Tab of Compliance Form.</t>
+  </si>
+  <si>
+    <t>Explained.  The application does not exclude any finding from the display even if the content are empty.</t>
   </si>
 </sst>
 </file>
@@ -440,7 +422,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]dd\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,17 +442,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <u/>
@@ -531,7 +502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -563,12 +534,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -582,20 +547,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <font>
         <strike val="0"/>
@@ -815,19 +767,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L31" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
-  <autoFilter ref="A1:L31"/>
-  <tableColumns count="12">
-    <tableColumn id="1" name="Serial No." dataDxfId="11"/>
-    <tableColumn id="2" name="Issue Date" dataDxfId="10"/>
-    <tableColumn id="3" name="Title" dataDxfId="9"/>
-    <tableColumn id="8" name="Issue Description" dataDxfId="8"/>
-    <tableColumn id="9" name="Category" dataDxfId="7"/>
-    <tableColumn id="4" name="Status" dataDxfId="6"/>
-    <tableColumn id="5" name="Action" dataDxfId="5"/>
-    <tableColumn id="6" name="Severity" dataDxfId="4"/>
-    <tableColumn id="10" name="Close Date" dataDxfId="3"/>
-    <tableColumn id="7" name="Column1" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K31" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11">
+  <autoFilter ref="A1:K31"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Serial No." dataDxfId="10"/>
+    <tableColumn id="2" name="Issue Date" dataDxfId="9"/>
+    <tableColumn id="3" name="Title" dataDxfId="8"/>
+    <tableColumn id="8" name="Issue Description" dataDxfId="7"/>
+    <tableColumn id="9" name="Category" dataDxfId="6"/>
+    <tableColumn id="4" name="Status" dataDxfId="5"/>
+    <tableColumn id="5" name="Action" dataDxfId="4"/>
+    <tableColumn id="6" name="Severity" dataDxfId="3"/>
+    <tableColumn id="10" name="Close Date" dataDxfId="2"/>
     <tableColumn id="11" name="Column2" dataDxfId="1"/>
     <tableColumn id="12" name="Column3" dataDxfId="0"/>
   </tableColumns>
@@ -1017,10 +968,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,14 +982,14 @@
     <col min="4" max="4" width="28.25" style="3" customWidth="1"/>
     <col min="5" max="5" width="14.75" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5" style="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.25" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.125" style="11" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="20.5" style="3" customWidth="1"/>
     <col min="12" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1066,24 +1017,21 @@
       <c r="I1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="14" t="s">
-        <v>102</v>
+      <c r="J1" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="5">
         <v>42809</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
@@ -1102,21 +1050,18 @@
         <v>11</v>
       </c>
       <c r="I2" s="10"/>
-      <c r="J2" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="180" x14ac:dyDescent="0.2">
+      <c r="J2" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="180" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="5">
         <v>42809</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="6" t="s">
@@ -1136,20 +1081,17 @@
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" ht="150" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="2" customFormat="1" ht="150" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="5">
         <v>42809</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="6" t="s">
@@ -1168,14 +1110,11 @@
         <v>11</v>
       </c>
       <c r="I4" s="10"/>
-      <c r="J4" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="J4" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1203,16 +1142,15 @@
       <c r="I5" s="10">
         <v>42809</v>
       </c>
-      <c r="J5" s="13"/>
-    </row>
-    <row r="6" spans="1:12" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:11" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="5">
         <v>42809</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -1231,21 +1169,18 @@
         <v>22</v>
       </c>
       <c r="I6" s="10"/>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="5">
         <v>42809</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -1264,21 +1199,18 @@
         <v>11</v>
       </c>
       <c r="I7" s="10"/>
-      <c r="J7" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="J7" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="5">
         <v>42809</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="6" t="s">
@@ -1298,20 +1230,17 @@
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="5">
         <v>42809</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="6" t="s">
@@ -1330,24 +1259,21 @@
         <v>11</v>
       </c>
       <c r="I9" s="10"/>
-      <c r="J9" s="4" t="s">
-        <v>108</v>
+      <c r="J9" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="5">
         <v>42809</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="14" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="6" t="s">
@@ -1366,19 +1292,21 @@
         <v>22</v>
       </c>
       <c r="I10" s="10"/>
-      <c r="J10" s="13"/>
-      <c r="L10" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="J10" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="5">
         <v>42809</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="15" t="s">
         <v>60</v>
       </c>
       <c r="D11" s="6" t="s">
@@ -1397,24 +1325,21 @@
         <v>11</v>
       </c>
       <c r="I11" s="10"/>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="2" t="s">
         <v>101</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="5">
         <v>42809</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="15" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="6" t="s">
@@ -1433,21 +1358,18 @@
         <v>11</v>
       </c>
       <c r="I12" s="10"/>
-      <c r="J12" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+      <c r="J12" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="5">
         <v>42809</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D13" s="6" t="s">
@@ -1467,23 +1389,20 @@
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K13" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:11" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="5">
         <v>42809</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D14" s="6" t="s">
@@ -1503,23 +1422,20 @@
       </c>
       <c r="I14" s="10"/>
       <c r="J14" s="2" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="5">
         <v>42809</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D15" s="6" t="s">
@@ -1539,23 +1455,20 @@
       </c>
       <c r="I15" s="10"/>
       <c r="J15" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="5">
         <v>42809</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D16" s="6" t="s">
@@ -1575,20 +1488,17 @@
       </c>
       <c r="I16" s="10"/>
       <c r="J16" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="2" customFormat="1" ht="180" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="2" customFormat="1" ht="180" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="5">
         <v>42809</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -1601,20 +1511,17 @@
         <v>9</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I17" s="10"/>
-      <c r="J17" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+      <c r="J17" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1640,19 +1547,18 @@
         <v>22</v>
       </c>
       <c r="I18" s="10"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="J18" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="5">
         <v>42809</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="15" t="s">
         <v>43</v>
       </c>
       <c r="D19" s="6" t="s">
@@ -1671,21 +1577,18 @@
         <v>22</v>
       </c>
       <c r="I19" s="10"/>
-      <c r="J19" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="J19" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="5">
         <v>42809</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="15" t="s">
         <v>45</v>
       </c>
       <c r="D20" s="6" t="s">
@@ -1704,21 +1607,18 @@
         <v>10</v>
       </c>
       <c r="I20" s="10"/>
-      <c r="J20" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" s="2" customFormat="1" ht="255" x14ac:dyDescent="0.2">
+      <c r="J20" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="2" customFormat="1" ht="255" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="5">
         <v>42809</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="15" t="s">
         <v>47</v>
       </c>
       <c r="D21" s="6" t="s">
@@ -1738,20 +1638,17 @@
       </c>
       <c r="I21" s="10"/>
       <c r="J21" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="5">
         <v>42809</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="15" t="s">
         <v>74</v>
       </c>
       <c r="D22" s="6" t="s">
@@ -1771,20 +1668,17 @@
         <v>101</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="5">
         <v>42809</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="15" t="s">
         <v>50</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -1800,21 +1694,18 @@
         <v>94</v>
       </c>
       <c r="I23" s="10"/>
-      <c r="J23" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.2">
+      <c r="J23" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="5">
         <v>42809</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="15" t="s">
         <v>51</v>
       </c>
       <c r="D24" s="6" t="s">
@@ -1834,20 +1725,17 @@
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" s="2" customFormat="1" ht="180" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="2" customFormat="1" ht="180" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="5">
         <v>42809</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="15" t="s">
         <v>52</v>
       </c>
       <c r="D25" s="6" t="s">
@@ -1866,12 +1754,11 @@
         <v>37</v>
       </c>
       <c r="I25" s="10"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="J25" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1898,13 +1785,10 @@
       </c>
       <c r="I26" s="10"/>
       <c r="J26" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1931,20 +1815,17 @@
       </c>
       <c r="I27" s="10"/>
       <c r="J27" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="5">
         <v>42809</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="15" t="s">
         <v>57</v>
       </c>
       <c r="D28" s="6" t="s">
@@ -1964,20 +1845,17 @@
       </c>
       <c r="I28" s="10"/>
       <c r="J28" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="5">
         <v>42809</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="15" t="s">
         <v>69</v>
       </c>
       <c r="D29" s="6" t="s">
@@ -1997,20 +1875,17 @@
       </c>
       <c r="I29" s="10"/>
       <c r="J29" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="5">
         <v>42809</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="15" t="s">
         <v>71</v>
       </c>
       <c r="D30" s="6" t="s">
@@ -2029,21 +1904,18 @@
         <v>11</v>
       </c>
       <c r="I30" s="10"/>
-      <c r="J30" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="J30" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="5">
         <v>42809</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="15" t="s">
         <v>72</v>
       </c>
       <c r="D31" s="6" t="s">
@@ -2062,11 +1934,8 @@
         <v>11</v>
       </c>
       <c r="I31" s="10"/>
-      <c r="J31" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>103</v>
+      <c r="J31" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>